<commit_message>
10 most common words on essay4
</commit_message>
<xml_diff>
--- a/Most_common_words.xlsx
+++ b/Most_common_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mexyr\Desktop\proj\OkCupid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\OneDrive\iTU\First Year Project\OkCupid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0B54A-E2C3-45A3-BEBF-450DA2CE7B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3D5217-827B-473B-956B-7CD74C46D6BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="2775" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <t xml:space="preserve"> m : f </t>
   </si>
   <si>
-    <t xml:space="preserve"> contains(get away) = True</t>
-  </si>
-  <si>
     <t>7.0 : 1.0</t>
   </si>
   <si>
@@ -688,9 +685,6 @@
     <t>contains(music except rap)</t>
   </si>
   <si>
-    <t>Etjnicity</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10.5 : 1.0</t>
   </si>
   <si>
@@ -1049,6 +1043,12 @@
   </si>
   <si>
     <t>f F1-Score: 0.6168810793850016</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> contains(get away)</t>
   </si>
 </sst>
 </file>
@@ -1506,57 +1506,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -1569,6 +1533,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1577,6 +1559,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,1151 +1861,1151 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="27.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
-    <col min="10" max="10" width="29.26953125" customWidth="1"/>
-    <col min="11" max="11" width="17.08984375" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" customWidth="1"/>
-    <col min="13" max="13" width="25.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8"/>
-      <c r="B1" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="20"/>
-      <c r="F1" s="42" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44"/>
-      <c r="J1" s="23" t="s">
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
+      <c r="J1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="31" t="s">
+      <c r="L2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" t="s">
+        <v>312</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" t="s">
+        <v>313</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="D6" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="I6" t="s">
+        <v>314</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I8" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>330</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>331</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" t="s">
+        <v>317</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
+        <v>332</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" t="s">
+        <v>311</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
+        <v>305</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="I15" t="s">
+        <v>306</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
+        <v>335</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="I16" t="s">
+        <v>307</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>336</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="I18" t="s">
+        <v>308</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" t="s">
+        <v>337</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I19" t="s">
+        <v>309</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" t="s">
+        <v>338</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" t="s">
+        <v>310</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" t="s">
+        <v>319</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I22" t="s">
+        <v>304</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" t="s">
         <v>320</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="F24" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="I24" t="s">
+        <v>298</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="I25" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="J25" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
+      <c r="B26" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" t="s">
+        <v>322</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="I26" t="s">
+        <v>300</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
+      <c r="B27" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="F27" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" t="s">
+        <v>323</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" t="s">
-        <v>328</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" t="s">
-        <v>314</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="H28" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="I28" t="s">
+        <v>301</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
+      <c r="B29" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>329</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="I5" t="s">
-        <v>315</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>330</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" t="s">
-        <v>316</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="L6" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="D29" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I29" t="s">
+        <v>302</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" t="s">
-        <v>331</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="I8" t="s">
-        <v>317</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="22" t="s">
+      <c r="D30" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" t="s">
+        <v>325</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="I30" t="s">
+        <v>303</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32"/>
+      <c r="B31" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" t="s">
-        <v>332</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="I9" t="s">
-        <v>318</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" t="s">
-        <v>333</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="I10" t="s">
-        <v>319</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="L10" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" t="s">
-        <v>334</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="I12" t="s">
-        <v>313</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L13" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="M13" s="17"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" t="s">
-        <v>335</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="I14" t="s">
-        <v>307</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L14" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>336</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I15" t="s">
-        <v>308</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L15" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" t="s">
-        <v>337</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="I16" t="s">
-        <v>309</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L16" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L17" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="M17" s="17"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" t="s">
-        <v>338</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="I18" t="s">
-        <v>310</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="36" t="s">
+      <c r="D31" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" t="s">
-        <v>339</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="I19" t="s">
-        <v>311</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L19" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" t="s">
-        <v>340</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="I20" t="s">
-        <v>312</v>
-      </c>
-      <c r="J20" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="L20" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="6"/>
-      <c r="B21" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="J21" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="K21" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="L21" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" t="s">
-        <v>321</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="I22" t="s">
-        <v>306</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="J23" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="L23" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="M23" s="17"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" t="s">
-        <v>322</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="H24" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="I24" t="s">
-        <v>300</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L24" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E25" t="s">
-        <v>323</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H25" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="I25" t="s">
-        <v>301</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L25" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" t="s">
-        <v>324</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H26" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="I26" t="s">
-        <v>302</v>
-      </c>
-      <c r="J26" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L26" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="L27" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="M27" s="17"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>211</v>
-      </c>
-      <c r="I28" t="s">
-        <v>303</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L28" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" t="s">
-        <v>326</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="H29" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="I29" t="s">
-        <v>304</v>
-      </c>
-      <c r="J29" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="K29" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="L29" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="M29" s="17" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" t="s">
-        <v>327</v>
-      </c>
-      <c r="F30" s="26" t="s">
+      <c r="F31" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="H31" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="G30" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="H30" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="I30" t="s">
-        <v>305</v>
-      </c>
-      <c r="J30" s="26" t="s">
+      <c r="J31" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="K31" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="K30" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="L30" s="27" t="s">
+      <c r="L31" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="M30" s="17" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="6"/>
-      <c r="B31" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="J31" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="K31" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="L31" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="M31" s="18"/>
+      <c r="M31" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="A12:A21"/>
     <mergeCell ref="A22:A31"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3020,27 +3020,27 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.54296875" customWidth="1"/>
-    <col min="3" max="3" width="62.36328125" customWidth="1"/>
-    <col min="4" max="4" width="58.54296875" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11"/>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3049,359 +3049,359 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="43"/>
+      <c r="B5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13"/>
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="44"/>
+      <c r="B11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+      <c r="B15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13"/>
-      <c r="B21" s="5" t="s">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="44"/>
+      <c r="B21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
+      <c r="B23" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+      <c r="B29" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="43"/>
+      <c r="B30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="44"/>
+      <c r="B31" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="13"/>
-      <c r="B31" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="14" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>